<commit_message>
Extracting Relevant data from previous data
Obtencion de diferentes datos utiles para calculos posteriores, se añadiran nuevos como probabilidades, desviaciones, etc
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,74 +434,104 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>posicion</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>nombre</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>puntos</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>partidos</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>ganados</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>empatados</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>perdidos</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>afavor</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>encontra</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Ha Ganado vs</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Ha perdido vs</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Ha empatado vs</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>golesAfavorUltimas5</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>golesEnContraUltimas5</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>maximos goles marcados ultimos5</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>minimos goles marcados ultimos5</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>maximos goles en contra ultimo5</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>minimos goles en contra ultimos5</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>media gol marcado ultimos5</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>media gol en contra ultimos5</t>
         </is>
       </c>
     </row>
@@ -560,6 +602,24 @@
       <c r="N2" t="n">
         <v>1</v>
       </c>
+      <c r="O2" t="n">
+        <v>3</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -628,6 +688,24 @@
       <c r="N3" t="n">
         <v>3</v>
       </c>
+      <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -696,6 +774,24 @@
       <c r="N4" t="n">
         <v>2</v>
       </c>
+      <c r="O4" t="n">
+        <v>3</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -764,6 +860,24 @@
       <c r="N5" t="n">
         <v>3</v>
       </c>
+      <c r="O5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -832,6 +946,24 @@
       <c r="N6" t="n">
         <v>4</v>
       </c>
+      <c r="O6" t="n">
+        <v>2</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -900,6 +1032,24 @@
       <c r="N7" t="n">
         <v>6</v>
       </c>
+      <c r="O7" t="n">
+        <v>2</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>3</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -968,6 +1118,24 @@
       <c r="N8" t="n">
         <v>8</v>
       </c>
+      <c r="O8" t="n">
+        <v>3</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1036,6 +1204,24 @@
       <c r="N9" t="n">
         <v>7</v>
       </c>
+      <c r="O9" t="n">
+        <v>4</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1104,6 +1290,24 @@
       <c r="N10" t="n">
         <v>3</v>
       </c>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1172,6 +1376,24 @@
       <c r="N11" t="n">
         <v>3</v>
       </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1191,7 +1413,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1206,7 +1428,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1216,7 +1438,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>31</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1226,19 +1448,37 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>['Villarreal', 'Barcelona']</t>
+          <t>['Villarreal', 'Barcelona', 'CÃ¡diz']</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>['Espanyol']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N12" t="n">
         <v>5</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1308,6 +1548,24 @@
       <c r="N13" t="n">
         <v>5</v>
       </c>
+      <c r="O13" t="n">
+        <v>4</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>3</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1376,6 +1634,24 @@
       <c r="N14" t="n">
         <v>5</v>
       </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>3</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1444,6 +1720,24 @@
       <c r="N15" t="n">
         <v>8</v>
       </c>
+      <c r="O15" t="n">
+        <v>3</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>2</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1453,64 +1747,82 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Espanyol</t>
+          <t>CÃ¡diz</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>21</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>17</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>33</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>['Getafe', 'Real Betis']</t>
+          <t>['Mallorca', 'Girona']</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>['AlmerÃ\xada']</t>
+          <t>['Sevilla', 'Athletic']</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>['Girona', 'Osasuna']</t>
+          <t>['Elche']</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N16" t="n">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>4</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1.2</v>
       </c>
     </row>
     <row r="17">
@@ -1521,7 +1833,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>Espanyol</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1536,49 +1848,67 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>24</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['Getafe', 'CÃ¡diz', 'Elche']</t>
+          <t>['Getafe', 'Real Betis']</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>['Girona', 'Barcelona']</t>
+          <t>['AlmerÃ\xada']</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Girona', 'Osasuna']</t>
         </is>
       </c>
       <c r="M17" t="n">
         <v>7</v>
       </c>
       <c r="N17" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>3</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1.4</v>
       </c>
     </row>
     <row r="18">
@@ -1589,19 +1919,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>20</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
       <c r="E18" t="inlineStr">
         <is>
           <t>5</t>
@@ -1609,44 +1939,62 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>21</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>29</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
+          <t>['Getafe', 'CÃ¡diz', 'Elche']</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>['Girona', 'Barcelona']</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>['CÃ¡diz', 'Real Valladolid', 'Real Madrid', 'Girona']</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>['AlmerÃ\xada']</t>
-        </is>
-      </c>
       <c r="M18" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N18" t="n">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="O18" t="n">
+        <v>3</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>3</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1.2</v>
       </c>
     </row>
     <row r="19">
@@ -1657,12 +2005,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CÃ¡diz</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1672,49 +2020,67 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>25</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>24</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['Valencia', 'Mallorca']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>['Sevilla', 'Athletic']</t>
+          <t>['CÃ¡diz', 'Real Valladolid', 'Real Madrid', 'Girona']</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>['Elche']</t>
+          <t>['AlmerÃ\xada']</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N19" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>2</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1.4</v>
       </c>
     </row>
     <row r="20">
@@ -1784,6 +2150,24 @@
       <c r="N20" t="n">
         <v>7</v>
       </c>
+      <c r="O20" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>2</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1851,6 +2235,24 @@
       </c>
       <c r="N21" t="n">
         <v>7</v>
+      </c>
+      <c r="O21" t="n">
+        <v>3</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>3</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>